<commit_message>
loginPage locators & read input data from excel
</commit_message>
<xml_diff>
--- a/testData/input.xlsx
+++ b/testData/input.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15240" windowHeight="2760"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15240" windowHeight="3105" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ValidLoginPage" sheetId="1" r:id="rId1"/>
     <sheet name="InvalidLoginPage" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:K7"/>
+  <oleSize ref="A1:G8"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>PassWord</t>
   </si>
@@ -56,13 +56,16 @@
     <t>test.sgautam@gmail.com</t>
   </si>
   <si>
-    <t>Gautam2123</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
     <t>Gautam@123</t>
+  </si>
+  <si>
+    <t>abc@gmail.com</t>
+  </si>
+  <si>
+    <t>Tester@123</t>
   </si>
 </sst>
 </file>
@@ -138,11 +141,12 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -416,7 +420,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -426,13 +430,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" customWidth="1"/>
     <col min="3" max="3" width="31.85546875" customWidth="1"/>
   </cols>
@@ -452,14 +456,15 @@
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
+      <c r="B2" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="C2" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -467,22 +472,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
     <col min="2" max="2" width="16.140625" customWidth="1"/>
     <col min="3" max="3" width="60.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -507,8 +512,9 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>13</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
@@ -517,6 +523,7 @@
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
@@ -525,6 +532,7 @@
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
@@ -533,20 +541,36 @@
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="2"/>
+      <c r="A7" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="B7" s="3" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>
     <hyperlink ref="A5" r:id="rId2"/>
-    <hyperlink ref="B7" r:id="rId3"/>
+    <hyperlink ref="B8" r:id="rId3"/>
+    <hyperlink ref="A7" r:id="rId4"/>
+    <hyperlink ref="B7" r:id="rId5"/>
+    <hyperlink ref="A8" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>